<commit_message>
delete method, image path and other stuff
</commit_message>
<xml_diff>
--- a/docs/Tables resulting from data dump.xlsx
+++ b/docs/Tables resulting from data dump.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Desktop\Main\03_Uni\WWI21DSA\02_Vorlesungen\03_Datenbanken I + II\bidbits\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FBA834C-D13B-48B5-B41F-86A315A883B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{516B5B67-6051-4E27-AA06-963E43F514E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32535" yWindow="2385" windowWidth="21600" windowHeight="11295" xr2:uid="{F6035A3A-C413-41D2-B014-F428AF47274A}"/>
+    <workbookView xWindow="4215" yWindow="1035" windowWidth="21600" windowHeight="11295" xr2:uid="{F6035A3A-C413-41D2-B014-F428AF47274A}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="84">
   <si>
     <t>Karen</t>
   </si>
@@ -252,6 +252,42 @@
   </si>
   <si>
     <t>receiver</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>image_path</t>
+  </si>
+  <si>
+    <t>time_left</t>
+  </si>
+  <si>
+    <t>highest_bid</t>
+  </si>
+  <si>
+    <t>Look what I found under my bed. It is golden, it is good.</t>
+  </si>
+  <si>
+    <t>items_status (View)</t>
+  </si>
+  <si>
+    <t>participated_auctions</t>
+  </si>
+  <si>
+    <t>won_auctions</t>
+  </si>
+  <si>
+    <t>average_rating</t>
+  </si>
+  <si>
+    <t>total_expenses</t>
+  </si>
+  <si>
+    <t>total_income</t>
+  </si>
+  <si>
+    <t>user_statistics (materialized view)</t>
   </si>
 </sst>
 </file>
@@ -283,7 +319,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -296,8 +332,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -320,17 +362,66 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -647,10 +738,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA7362D2-028B-4961-98F8-B5562DC92A16}">
-  <dimension ref="B2:AX7"/>
+  <dimension ref="B2:BG17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H18" activeCellId="1" sqref="AX30 H18"/>
+    <sheetView tabSelected="1" topLeftCell="AI1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AN8" sqref="AN8:AR17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -693,9 +784,21 @@
     <col min="43" max="43" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="44" max="44" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="45" max="45" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="50.7109375" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="107" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:50" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:59" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="5" t="s">
         <v>64</v>
       </c>
@@ -748,8 +851,24 @@
       <c r="AQ2" s="5"/>
       <c r="AR2" s="5"/>
       <c r="AS2" s="5"/>
+      <c r="AU2" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="AV2" s="8"/>
+      <c r="AW2" s="8"/>
+      <c r="AX2" s="8"/>
+      <c r="AY2" s="8"/>
+      <c r="AZ2" s="9"/>
+      <c r="BB2" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="BC2" s="6"/>
+      <c r="BD2" s="6"/>
+      <c r="BE2" s="6"/>
+      <c r="BF2" s="6"/>
+      <c r="BG2" s="6"/>
     </row>
-    <row r="3" spans="2:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:59" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>19</v>
       </c>
@@ -862,14 +981,46 @@
         <v>33</v>
       </c>
       <c r="AS3" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AU3"/>
-      <c r="AV3"/>
-      <c r="AW3"/>
-      <c r="AX3"/>
+        <v>54</v>
+      </c>
+      <c r="AU3" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="AV3" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="AW3" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="AX3" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="AY3" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="AZ3" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="BB3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="BC3" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="BD3" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="BE3" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="BF3" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="BG3" s="3" t="s">
+        <v>82</v>
+      </c>
     </row>
-    <row r="4" spans="2:50" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:59" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
@@ -982,8 +1133,40 @@
       <c r="AS4" s="1">
         <v>3</v>
       </c>
+      <c r="AU4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AV4" s="1">
+        <v>1</v>
+      </c>
+      <c r="AW4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AX4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AY4" s="1">
+        <v>17</v>
+      </c>
+      <c r="AZ4" s="1">
+        <v>24</v>
+      </c>
+      <c r="BB4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="BC4" s="1">
+        <v>1</v>
+      </c>
+      <c r="BD4" s="1"/>
+      <c r="BE4" s="1">
+        <v>1</v>
+      </c>
+      <c r="BF4" s="1"/>
+      <c r="BG4" s="1">
+        <v>42</v>
+      </c>
     </row>
-    <row r="5" spans="2:50" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:59" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
@@ -1081,8 +1264,40 @@
       <c r="AM5" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="AU5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AV5" s="1">
+        <v>2</v>
+      </c>
+      <c r="AW5" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AX5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AY5" s="1">
+        <v>14</v>
+      </c>
+      <c r="AZ5" s="1">
+        <v>1300000000</v>
+      </c>
+      <c r="BB5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="BC5" s="1">
+        <v>2</v>
+      </c>
+      <c r="BD5" s="1"/>
+      <c r="BE5" s="1">
+        <v>10</v>
+      </c>
+      <c r="BF5" s="1">
+        <v>42</v>
+      </c>
+      <c r="BG5" s="1"/>
     </row>
-    <row r="6" spans="2:50" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:59" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>13</v>
       </c>
@@ -1164,8 +1379,38 @@
       <c r="AF6" s="1">
         <v>1</v>
       </c>
+      <c r="AU6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AV6" s="1">
+        <v>3</v>
+      </c>
+      <c r="AW6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AX6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AY6" s="1">
+        <v>-13</v>
+      </c>
+      <c r="AZ6" s="1">
+        <v>20</v>
+      </c>
+      <c r="BB6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="BC6" s="1">
+        <v>2</v>
+      </c>
+      <c r="BD6" s="1">
+        <v>1</v>
+      </c>
+      <c r="BE6" s="1"/>
+      <c r="BF6" s="1"/>
+      <c r="BG6" s="1"/>
     </row>
-    <row r="7" spans="2:50" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:59" x14ac:dyDescent="0.25">
       <c r="U7" s="1">
         <v>4</v>
       </c>
@@ -1175,9 +1420,78 @@
       <c r="W7" s="1" t="s">
         <v>51</v>
       </c>
+      <c r="Y7" s="1">
+        <v>4</v>
+      </c>
+      <c r="Z7" s="1">
+        <v>16</v>
+      </c>
+      <c r="AA7" s="2">
+        <v>43835.799560185187</v>
+      </c>
+      <c r="AB7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC7" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="2:59" x14ac:dyDescent="0.25">
+      <c r="Y8" s="1">
+        <v>5</v>
+      </c>
+      <c r="Z8" s="1">
+        <v>18</v>
+      </c>
+      <c r="AA8" s="2">
+        <v>43839.842268518521</v>
+      </c>
+      <c r="AB8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC8" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="2:59" x14ac:dyDescent="0.25">
+      <c r="Y9" s="1">
+        <v>6</v>
+      </c>
+      <c r="Z9" s="1">
+        <v>19</v>
+      </c>
+      <c r="AA9" s="2">
+        <v>43835.799560185187</v>
+      </c>
+      <c r="AB9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC9" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="2:59" x14ac:dyDescent="0.25">
+      <c r="AO11" s="4"/>
+    </row>
+    <row r="12" spans="2:59" x14ac:dyDescent="0.25">
+      <c r="AO12" s="4"/>
+    </row>
+    <row r="13" spans="2:59" x14ac:dyDescent="0.25">
+      <c r="AO13" s="4"/>
+    </row>
+    <row r="14" spans="2:59" x14ac:dyDescent="0.25">
+      <c r="AO14" s="4"/>
+    </row>
+    <row r="16" spans="2:59" x14ac:dyDescent="0.25">
+      <c r="AO16" s="4"/>
+    </row>
+    <row r="17" spans="41:41" x14ac:dyDescent="0.25">
+      <c r="AO17" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="9">
+    <mergeCell ref="AU2:AZ2"/>
+    <mergeCell ref="BB2:BG2"/>
     <mergeCell ref="AO2:AS2"/>
     <mergeCell ref="B2:I2"/>
     <mergeCell ref="K2:S2"/>

</xml_diff>

<commit_message>
ich push push push
</commit_message>
<xml_diff>
--- a/docs/Tables resulting from data dump.xlsx
+++ b/docs/Tables resulting from data dump.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Desktop\Main\03_Uni\WWI21DSA\02_Vorlesungen\03_Datenbanken I + II\bidbits\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20B1B7AB-0683-4E16-A242-3127EA022D8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A3E7683-2F8D-457D-A8DF-C9AC3122FD43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26970" yWindow="1200" windowWidth="21600" windowHeight="11295" xr2:uid="{F6035A3A-C413-41D2-B014-F428AF47274A}"/>
+    <workbookView xWindow="-27120" yWindow="1380" windowWidth="21600" windowHeight="11295" xr2:uid="{F6035A3A-C413-41D2-B014-F428AF47274A}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="86">
   <si>
     <t>Karen</t>
   </si>
@@ -288,6 +288,12 @@
   </si>
   <si>
     <t>user_statistics (materialized view)</t>
+  </si>
+  <si>
+    <t>highest bidder</t>
+  </si>
+  <si>
+    <t>seller</t>
   </si>
 </sst>
 </file>
@@ -403,7 +409,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -424,6 +430,11 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -738,10 +749,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA7362D2-028B-4961-98F8-B5562DC92A16}">
-  <dimension ref="B2:BG17"/>
+  <dimension ref="B2:BI17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AX1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="BF3" sqref="BF3"/>
+    <sheetView tabSelected="1" topLeftCell="S1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="BC3" sqref="BC3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -790,15 +801,16 @@
     <col min="50" max="50" width="107" bestFit="1" customWidth="1"/>
     <col min="51" max="51" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="52" max="52" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="53" max="54" width="11.7109375" customWidth="1"/>
+    <col min="56" max="56" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:59" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:61" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="9" t="s">
         <v>64</v>
       </c>
@@ -859,16 +871,18 @@
       <c r="AX2" s="6"/>
       <c r="AY2" s="6"/>
       <c r="AZ2" s="7"/>
-      <c r="BB2" s="8" t="s">
+      <c r="BA2" s="10"/>
+      <c r="BB2" s="10"/>
+      <c r="BD2" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="BC2" s="8"/>
-      <c r="BD2" s="8"/>
       <c r="BE2" s="8"/>
       <c r="BF2" s="8"/>
       <c r="BG2" s="8"/>
+      <c r="BH2" s="8"/>
+      <c r="BI2" s="8"/>
     </row>
-    <row r="3" spans="2:59" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:61" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>19</v>
       </c>
@@ -1001,26 +1015,32 @@
       <c r="AZ3" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="BB3" s="3" t="s">
+      <c r="BA3" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="BB3" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="BD3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="BC3" s="3" t="s">
+      <c r="BE3" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="BD3" s="3" t="s">
+      <c r="BF3" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="BE3" s="3" t="s">
+      <c r="BG3" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="BF3" s="3" t="s">
+      <c r="BH3" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="BG3" s="3" t="s">
+      <c r="BI3" s="3" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="4" spans="2:59" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:61" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
@@ -1151,22 +1171,24 @@
       <c r="AZ4" s="1">
         <v>24</v>
       </c>
-      <c r="BB4" s="1" t="s">
+      <c r="BA4" s="12"/>
+      <c r="BB4" s="12"/>
+      <c r="BD4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="BC4" s="1">
-        <v>1</v>
-      </c>
-      <c r="BD4" s="1"/>
       <c r="BE4" s="1">
         <v>1</v>
       </c>
       <c r="BF4" s="1"/>
       <c r="BG4" s="1">
+        <v>1</v>
+      </c>
+      <c r="BH4" s="1"/>
+      <c r="BI4" s="1">
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="2:59" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:61" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
@@ -1282,22 +1304,24 @@
       <c r="AZ5" s="1">
         <v>1300000000</v>
       </c>
-      <c r="BB5" s="1" t="s">
+      <c r="BA5" s="12"/>
+      <c r="BB5" s="12"/>
+      <c r="BD5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="BC5" s="1">
+      <c r="BE5" s="1">
         <v>2</v>
       </c>
-      <c r="BD5" s="1"/>
-      <c r="BE5" s="1">
+      <c r="BF5" s="1"/>
+      <c r="BG5" s="1">
         <v>10</v>
       </c>
-      <c r="BF5" s="1">
+      <c r="BH5" s="1">
         <v>42</v>
       </c>
-      <c r="BG5" s="1"/>
+      <c r="BI5" s="1"/>
     </row>
-    <row r="6" spans="2:59" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:61" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>13</v>
       </c>
@@ -1397,20 +1421,22 @@
       <c r="AZ6" s="1">
         <v>20</v>
       </c>
-      <c r="BB6" s="1" t="s">
+      <c r="BA6" s="12"/>
+      <c r="BB6" s="12"/>
+      <c r="BD6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="BC6" s="1">
+      <c r="BE6" s="1">
         <v>2</v>
       </c>
-      <c r="BD6" s="1">
+      <c r="BF6" s="1">
         <v>1</v>
       </c>
-      <c r="BE6" s="1"/>
-      <c r="BF6" s="1"/>
       <c r="BG6" s="1"/>
+      <c r="BH6" s="1"/>
+      <c r="BI6" s="1"/>
     </row>
-    <row r="7" spans="2:59" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:61" x14ac:dyDescent="0.25">
       <c r="U7" s="1">
         <v>4</v>
       </c>
@@ -1436,7 +1462,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="2:59" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:61" x14ac:dyDescent="0.25">
       <c r="Y8" s="1">
         <v>5</v>
       </c>
@@ -1453,7 +1479,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="2:59" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:61" x14ac:dyDescent="0.25">
       <c r="Y9" s="1">
         <v>6</v>
       </c>
@@ -1470,19 +1496,19 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="2:59" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:61" x14ac:dyDescent="0.25">
       <c r="AO11" s="4"/>
     </row>
-    <row r="12" spans="2:59" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:61" x14ac:dyDescent="0.25">
       <c r="AO12" s="4"/>
     </row>
-    <row r="13" spans="2:59" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:61" x14ac:dyDescent="0.25">
       <c r="AO13" s="4"/>
     </row>
-    <row r="14" spans="2:59" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:61" x14ac:dyDescent="0.25">
       <c r="AO14" s="4"/>
     </row>
-    <row r="16" spans="2:59" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:61" x14ac:dyDescent="0.25">
       <c r="AO16" s="4"/>
     </row>
     <row r="17" spans="41:41" x14ac:dyDescent="0.25">
@@ -1491,7 +1517,7 @@
   </sheetData>
   <mergeCells count="9">
     <mergeCell ref="AU2:AZ2"/>
-    <mergeCell ref="BB2:BG2"/>
+    <mergeCell ref="BD2:BI2"/>
     <mergeCell ref="AO2:AS2"/>
     <mergeCell ref="B2:I2"/>
     <mergeCell ref="K2:S2"/>

</xml_diff>